<commit_message>
add list of projects on map when category is selected
</commit_message>
<xml_diff>
--- a/app/data/src/projectlist.xlsx
+++ b/app/data/src/projectlist.xlsx
@@ -1616,9 +1616,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="69" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1626,7 +1626,8 @@
     <col min="1" max="1" width="53" style="4" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="28.33203125" style="4" customWidth="1"/>
-    <col min="4" max="5" width="23.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="34.1640625" style="4" customWidth="1"/>
     <col min="6" max="6" width="47.83203125" style="6" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" style="6" customWidth="1"/>
     <col min="8" max="8" width="19.83203125" style="5" customWidth="1"/>

</xml_diff>